<commit_message>
dsa dp and sql
</commit_message>
<xml_diff>
--- a/java/LC_DP_and_DP_GM.xlsx
+++ b/java/LC_DP_and_DP_GM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCB74E8-FDF4-49DD-ADA3-153585D2C5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533BA815-2554-484C-8A45-D749395520F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Question</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>General 2D DP. We accumulate paths. Conditions to check are out of bounds and goal state. Need to use memoization or bottom-up to get accepted.</t>
+  </si>
+  <si>
+    <t>646. Maximum Length of Pair Chain</t>
+  </si>
+  <si>
+    <t>The optimal is the Greedy solution. House Robber variation. Take/Not Take. Based on the conditions, we need to skip, but if conditions are met, we need to iterate within the recursive function to find maxChain of max(maxChain, 1+solve) (take and not take for the rest of the array). The return is then the max of maxChain and solve(i+1) (not take). Remember the Java 8 lambda sort for sorting a 2d array: Arrays.sort(pairs, (a,b) -&gt; Integer.compare(a[0], b[0])); You need memoization atleast to pass TLE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/maximum-length-of-pair-chain/solutions/745935/java-solution-recursion-memoziation/?envType=study-plan-v2&amp;envId=dynamic-programming </t>
   </si>
 </sst>
 </file>
@@ -515,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,6 +725,23 @@
         <v>43</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{436C69DA-27D6-403C-8212-6636E4851942}"/>
@@ -728,6 +754,7 @@
     <hyperlink ref="E9" r:id="rId8" xr:uid="{ECCDD114-4E77-4057-8011-A287BC1556F0}"/>
     <hyperlink ref="E10" r:id="rId9" xr:uid="{DDCD26F3-AE01-4A79-BD34-1966942BA4DF}"/>
     <hyperlink ref="E11" r:id="rId10" xr:uid="{AFAC3A84-8B5F-4BD6-A701-1330B27367F1}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{C802FC15-EDAE-46F3-9E5B-3F333D6D5487}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa graphs, pandas, sql
</commit_message>
<xml_diff>
--- a/java/LC_DP_and_DP_GM.xlsx
+++ b/java/LC_DP_and_DP_GM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533BA815-2554-484C-8A45-D749395520F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF62F314-104E-4F24-A988-82276FA8CE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Question</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/maximum-length-of-pair-chain/solutions/745935/java-solution-recursion-memoziation/?envType=study-plan-v2&amp;envId=dynamic-programming </t>
+  </si>
+  <si>
+    <t>1020. Number of Enclaves</t>
+  </si>
+  <si>
+    <t>Matrix Graphs</t>
+  </si>
+  <si>
+    <t>Flood fill from the edges. DFS from any 1s on the edges and mark them as 0, then to another pass to count the remaining 1s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/number-of-enclaves/solutions/3388131/python-java-c-simple-solution-easy-to-understand/?envType=study-plan-v2&amp;envId=graph-theory </t>
   </si>
 </sst>
 </file>
@@ -524,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,6 +754,23 @@
         <v>47</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{436C69DA-27D6-403C-8212-6636E4851942}"/>
@@ -755,6 +784,7 @@
     <hyperlink ref="E10" r:id="rId9" xr:uid="{DDCD26F3-AE01-4A79-BD34-1966942BA4DF}"/>
     <hyperlink ref="E11" r:id="rId10" xr:uid="{AFAC3A84-8B5F-4BD6-A701-1330B27367F1}"/>
     <hyperlink ref="E12" r:id="rId11" xr:uid="{C802FC15-EDAE-46F3-9E5B-3F333D6D5487}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{6A4E6840-FF66-4239-864F-B22329F7C640}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>